<commit_message>
add a bunch of data files
</commit_message>
<xml_diff>
--- a/school/SelectedPopulations.xlsx
+++ b/school/SelectedPopulations.xlsx
@@ -11609,7 +11609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1854"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
@@ -81910,10 +81912,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="K5:L5"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>

</xml_diff>